<commit_message>
add in kill switch and feedback api...
</commit_message>
<xml_diff>
--- a/features/backlog/android/enable_disable_notification_settings.xlsx
+++ b/features/backlog/android/enable_disable_notification_settings.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E065C30-CCD2-48DE-B5F8-DF224062F940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30744C1D-069A-4407-861A-447194575FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="notifications" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="119">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -275,6 +275,139 @@
   <si>
     <t>Toggle notifications when the device is in offline mode. Confirm that the app handles this scenario gracefully.</t>
   </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find the notification toogle button</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and observe the notification toogle button</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and tap on the notification toogle button</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and disable the notification toogle button</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and disable the notification toogle button
+5. close the app.
+6. open the app.</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and enable the notification toogle button</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and enable the notification toogle button
+5. try to enable again</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. login to the app using premium users
+3. tap on the settings
+4. find and disable the notification toogle button
+5. try to disable again</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-023</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-024</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-025</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-026</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-027</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-028</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-029</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-030</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-031</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-032</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-033</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-034</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-035</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-036</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-037</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-038</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-039</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-040</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-041</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-042</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-043</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-044</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-045</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-046</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-047</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-048</t>
+  </si>
+  <si>
+    <t>SYMENADISNOT-049</t>
+  </si>
 </sst>
 </file>
 
@@ -466,9 +599,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1358,8 +1493,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1475,7 +1610,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1486,7 +1621,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>8</v>
@@ -1517,7 +1652,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1528,7 +1663,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>8</v>
@@ -1555,7 +1690,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
@@ -1566,7 +1701,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>8</v>
@@ -1593,7 +1728,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1604,7 +1739,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>8</v>
@@ -1631,7 +1766,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -1642,7 +1777,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>8</v>
@@ -1669,7 +1804,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
@@ -1680,7 +1815,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>8</v>
@@ -1707,7 +1842,7 @@
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1718,7 +1853,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>8</v>
@@ -1745,7 +1880,7 @@
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1756,7 +1891,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>8</v>
@@ -1783,7 +1918,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
@@ -1794,7 +1929,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>8</v>
@@ -1821,7 +1956,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>40</v>
       </c>
@@ -1832,7 +1967,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>8</v>
@@ -1859,7 +1994,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
@@ -1870,7 +2005,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>8</v>
@@ -1897,7 +2032,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
@@ -1908,7 +2043,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>8</v>
@@ -1935,7 +2070,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>43</v>
       </c>
@@ -1946,7 +2081,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>8</v>
@@ -1973,7 +2108,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>44</v>
       </c>
@@ -2011,7 +2146,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>45</v>
       </c>
@@ -2049,7 +2184,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>46</v>
       </c>
@@ -2087,7 +2222,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>53</v>
       </c>
@@ -2125,7 +2260,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
@@ -2163,7 +2298,7 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -2201,7 +2336,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
@@ -2239,7 +2374,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
@@ -2277,7 +2412,7 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>46</v>
       </c>
@@ -2315,7 +2450,7 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
@@ -2353,7 +2488,7 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>48</v>
       </c>
@@ -2391,7 +2526,7 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>49</v>
       </c>
@@ -2429,7 +2564,7 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>50</v>
       </c>
@@ -2467,7 +2602,7 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>51</v>
       </c>
@@ -2505,9 +2640,9 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>7</v>
@@ -2543,9 +2678,9 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>7</v>
@@ -2581,9 +2716,9 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>7</v>
@@ -2619,9 +2754,9 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>7</v>
@@ -2657,9 +2792,9 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>7</v>
@@ -2695,9 +2830,9 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>7</v>
@@ -2733,9 +2868,9 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>7</v>
@@ -2771,9 +2906,9 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>7</v>
@@ -2809,9 +2944,9 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>7</v>
@@ -2847,9 +2982,9 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>7</v>
@@ -2885,9 +3020,9 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>7</v>
@@ -2923,9 +3058,9 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>7</v>
@@ -2961,9 +3096,9 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>7</v>
@@ -2999,9 +3134,9 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>7</v>
@@ -3037,9 +3172,9 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>7</v>
@@ -3075,9 +3210,9 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>7</v>
@@ -3113,9 +3248,9 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>7</v>
@@ -3151,9 +3286,9 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>7</v>
@@ -3189,9 +3324,9 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>7</v>
@@ -3227,9 +3362,9 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>7</v>
@@ -3265,9 +3400,9 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>7</v>
@@ -3303,9 +3438,9 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>7</v>
@@ -3341,9 +3476,9 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>7</v>
@@ -3379,9 +3514,9 @@
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
     </row>
-    <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>7</v>
@@ -3417,9 +3552,9 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>7</v>
@@ -3455,9 +3590,9 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>7</v>
@@ -3493,9 +3628,9 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>7</v>

</xml_diff>